<commit_message>
Added column for LinearSVC benchmark
</commit_message>
<xml_diff>
--- a/specialists_benchmark.xlsx
+++ b/specialists_benchmark.xlsx
@@ -512,7 +512,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.2" defaultRowHeight="15"/>
@@ -558,7 +558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -583,8 +583,11 @@
       <c r="H2">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -609,8 +612,11 @@
       <c r="H3">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -635,8 +641,11 @@
       <c r="H4">
         <v>0.58</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -661,8 +670,11 @@
       <c r="H5">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -687,8 +699,11 @@
       <c r="H6">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -713,8 +728,11 @@
       <c r="H7">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -739,8 +757,11 @@
       <c r="H8">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -765,8 +786,11 @@
       <c r="H9">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -791,8 +815,11 @@
       <c r="H10">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -817,8 +844,11 @@
       <c r="H11">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -843,8 +873,11 @@
       <c r="H12">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -869,8 +902,11 @@
       <c r="H13">
         <v>0.76</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -889,8 +925,11 @@
       <c r="H14">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -915,8 +954,11 @@
       <c r="H15">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -941,8 +983,11 @@
       <c r="H16">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -967,8 +1012,11 @@
       <c r="H17">
         <v>0.57</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -993,8 +1041,11 @@
       <c r="H18">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1016,8 +1067,11 @@
       <c r="H19">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1042,8 +1096,11 @@
       <c r="H20">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1067,6 +1124,9 @@
       </c>
       <c r="H21">
         <v>0.61</v>
+      </c>
+      <c r="I21">
+        <v>0.74</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1101,9 +1161,9 @@
         <f>AVERAGE(H2:H21)</f>
         <v>0.71</v>
       </c>
-      <c r="I22" t="e">
+      <c r="I22">
         <f>AVERAGE(I2:I21)</f>
-        <v>#DIV/0!</v>
+        <v>0.7955</v>
       </c>
       <c r="J22" t="e">
         <f>AVERAGE(J2:J21)</f>

</xml_diff>

<commit_message>
Added column for CNN benchmark
</commit_message>
<xml_diff>
--- a/specialists_benchmark.xlsx
+++ b/specialists_benchmark.xlsx
@@ -44,7 +44,7 @@
     <t>LinSVC</t>
   </si>
   <si>
-    <t>CNN</t>
+    <t>CNN logloss</t>
   </si>
   <si>
     <t>Protists</t>
@@ -512,7 +512,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.2" defaultRowHeight="15"/>
@@ -524,6 +524,7 @@
     <col min="5" max="5" width="10.3" customWidth="1"/>
     <col min="6" max="6" width="12.3" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="10" max="10" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -558,7 +559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -586,8 +587,11 @@
       <c r="I2">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -615,8 +619,11 @@
       <c r="I3">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>17.76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -644,8 +651,11 @@
       <c r="I4">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -673,8 +683,11 @@
       <c r="I5">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <v>4.79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -702,8 +715,11 @@
       <c r="I6">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -731,8 +747,11 @@
       <c r="I7">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -760,8 +779,11 @@
       <c r="I8">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>8.42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -789,8 +811,11 @@
       <c r="I9">
         <v>0.79</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>15.07</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -818,8 +843,11 @@
       <c r="I10">
         <v>0.83</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <v>11.97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -847,8 +875,11 @@
       <c r="I11">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -876,8 +907,11 @@
       <c r="I12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12">
+        <v>4.79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -905,8 +939,11 @@
       <c r="I13">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13">
+        <v>9.88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -928,8 +965,11 @@
       <c r="I14">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -957,8 +997,11 @@
       <c r="I15">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -986,8 +1029,11 @@
       <c r="I16">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16">
+        <v>13.63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1015,8 +1061,11 @@
       <c r="I17">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17">
+        <v>0.829</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1044,8 +1093,11 @@
       <c r="I18">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18">
+        <v>15.69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1070,8 +1122,11 @@
       <c r="I19">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1099,8 +1154,11 @@
       <c r="I20">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20">
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1127,6 +1185,9 @@
       </c>
       <c r="I21">
         <v>0.74</v>
+      </c>
+      <c r="J21">
+        <v>15.42</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1165,9 +1226,9 @@
         <f>AVERAGE(I2:I21)</f>
         <v>0.7955</v>
       </c>
-      <c r="J22" t="e">
+      <c r="J22">
         <f>AVERAGE(J2:J21)</f>
-        <v>#DIV/0!</v>
+        <v>8.32945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>